<commit_message>
Updated Excel Final PSB
</commit_message>
<xml_diff>
--- a/public/Excel Templates/CAF-DH.xlsx
+++ b/public/Excel Templates/CAF-DH.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HRIS\hris_api\public\Excel Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813B74CA-F37B-4D1B-99C6-418D5AE09D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8A66E213-2698-45A8-B21E-88CC94A2EFF7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Permanent" sheetId="1" r:id="rId1"/>
@@ -34,7 +33,7 @@
     <definedName name="Position">#REF!</definedName>
     <definedName name="TRAINING">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="36">
   <si>
     <t>C O M P A R A T I V E    A S S E S S M E N T   F O R M</t>
   </si>
@@ -150,89 +149,13 @@
     <t>NAME OF CANDIDATE</t>
   </si>
   <si>
-    <t>BRIAN A. CAMHIT</t>
-  </si>
-  <si>
-    <t>RUBEN E. PAOAD</t>
-  </si>
-  <si>
-    <t>FLORENCIO V. BENTREZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provincial Human Resource </t>
-  </si>
-  <si>
-    <t>SP Member &amp; Committee Chairman</t>
-  </si>
-  <si>
-    <t>SP Member &amp; Committee Chairman on</t>
-  </si>
-  <si>
-    <t>Management &amp; Development Officer</t>
-  </si>
-  <si>
-    <t>on Labor &amp; Employment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personnel Administration </t>
-  </si>
-  <si>
     <t>DATE OF EFFECTIVITY</t>
-  </si>
-  <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>Temporary Presiding Officer</t>
   </si>
   <si>
     <t>APPROVED:</t>
   </si>
   <si>
-    <t>CHARLIE B. PINAS</t>
-  </si>
-  <si>
-    <t>MELIARAZON F. DULAY, MD, FPOGS</t>
-  </si>
-  <si>
-    <t>FREZILLA M. SIMEON</t>
-  </si>
-  <si>
-    <t>MELCHOR D. DICLAS, MD</t>
-  </si>
-  <si>
-    <r>
-      <t>BPGEA 2</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>nd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Level Representative</t>
-    </r>
-  </si>
-  <si>
-    <t>PHO I / Acting Chief of Hospital III</t>
-  </si>
-  <si>
-    <t>Executive Assistant III</t>
-  </si>
-  <si>
     <t>Provincial Governor</t>
-  </si>
-  <si>
-    <t>PGO - Benguet provides equal employment opportunities to its employees and applicants regardless of gender, sexual orientation, age, religion, ethnicity, status, indigenous group or physical handicaps.</t>
   </si>
   <si>
     <t xml:space="preserve">QUALIFICATION STANDARDS </t>
@@ -264,17 +187,20 @@
   <si>
     <t>COMPETENCIES</t>
   </si>
+  <si>
+    <t>This agency Benguet provides equal employment opportunities to its employees and applicants regardless of gender, sexual orientation, age, religion, ethnicity, status, indigenous group or physical handicaps.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$₱-464]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,12 +263,6 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -606,8 +526,8 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -698,11 +618,11 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -759,277 +679,277 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma 2" xfId="3" xr:uid="{4DAE9455-D5EC-4039-96E0-91C6C32A4238}"/>
+    <cellStyle name="Comma 2" xfId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{78454837-B544-42D8-BE24-246D40853A45}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -1151,7 +1071,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="perm"/>
@@ -1232,7 +1152,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="PDO I"/>
@@ -1590,14 +1510,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39441AF3-F7FD-4DC8-94BA-EE337756DF43}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1625,63 +1545,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
       <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1691,13 +1611,13 @@
       <c r="N3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="9"/>
@@ -1706,65 +1626,65 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
       <c r="L4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="M4" s="30"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
+      <c r="A5" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
       <c r="L6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
       <c r="O6" s="5"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="5"/>
@@ -1772,24 +1692,24 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
       <c r="L7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -1839,103 +1759,103 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="1:21" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="53" t="s">
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="55" t="s">
+      <c r="J10" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="53" t="s">
+      <c r="K10" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="49"/>
-      <c r="O10" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" s="53" t="s">
+      <c r="M10" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="70"/>
+      <c r="O10" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="T10" s="59" t="s">
+      <c r="T10" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="U10" s="61" t="s">
+      <c r="U10" s="65" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="26.25" thickBot="1">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="52"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="72"/>
       <c r="O11" s="11" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="62"/>
+        <v>32</v>
+      </c>
+      <c r="R11" s="68"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="66"/>
     </row>
     <row r="12" spans="1:21" s="35" customFormat="1">
       <c r="A12" s="33">
         <v>1</v>
       </c>
       <c r="B12" s="34"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="75"/>
-      <c r="T12" s="76"/>
-      <c r="U12" s="77"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="93"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="45"/>
     </row>
     <row r="13" spans="1:21" s="35" customFormat="1">
       <c r="A13" s="36"/>
@@ -1943,27 +1863,27 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="87"/>
-      <c r="Q13" s="87"/>
-      <c r="R13" s="87"/>
-      <c r="S13" s="88"/>
-      <c r="T13" s="89"/>
-      <c r="U13" s="90"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="52"/>
+      <c r="U13" s="53"/>
     </row>
     <row r="14" spans="1:21" s="35" customFormat="1">
       <c r="A14" s="36"/>
@@ -1971,27 +1891,27 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="87"/>
-      <c r="Q14" s="87"/>
-      <c r="R14" s="87"/>
-      <c r="S14" s="88"/>
-      <c r="T14" s="89"/>
-      <c r="U14" s="91"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="54"/>
     </row>
     <row r="15" spans="1:21" s="35" customFormat="1">
       <c r="A15" s="36"/>
@@ -1999,50 +1919,50 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="85"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87"/>
-      <c r="R15" s="87"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="91"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="52"/>
+      <c r="U15" s="54"/>
     </row>
     <row r="16" spans="1:21" s="35" customFormat="1">
       <c r="A16" s="36"/>
       <c r="B16" s="37"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="84"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="86"/>
-      <c r="P16" s="87"/>
-      <c r="Q16" s="87"/>
-      <c r="R16" s="87"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="89"/>
-      <c r="U16" s="91"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="88"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="52"/>
+      <c r="U16" s="54"/>
     </row>
     <row r="17" spans="1:21" ht="16.5" thickBot="1">
       <c r="A17" s="32"/>
@@ -2050,25 +1970,25 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="97"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="99"/>
-      <c r="M17" s="100"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="105"/>
-      <c r="U17" s="106"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="61"/>
+      <c r="U17" s="62"/>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="5" t="s">
@@ -2178,13 +2098,13 @@
       <c r="L22" s="10"/>
       <c r="M22" s="13"/>
       <c r="N22" s="5"/>
-      <c r="O22" s="41" t="s">
+      <c r="O22" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="84"/>
+      <c r="R22" s="84"/>
+      <c r="S22" s="84"/>
       <c r="U22" s="14"/>
     </row>
     <row r="23" spans="1:21">
@@ -2207,26 +2127,20 @@
       <c r="U23" s="14"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="N24" s="40"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="86"/>
       <c r="O24" s="19"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
@@ -2235,26 +2149,20 @@
       <c r="U24" s="14"/>
     </row>
     <row r="25" spans="1:21" ht="16.5" thickBot="1">
-      <c r="A25" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="N25" s="39"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="103"/>
+      <c r="J25" s="103"/>
+      <c r="K25" s="103"/>
+      <c r="L25" s="103"/>
+      <c r="M25" s="103"/>
+      <c r="N25" s="103"/>
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="20"/>
@@ -2264,57 +2172,45 @@
       <c r="U25" s="14"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="N26" s="39"/>
-      <c r="O26" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
+      <c r="A26" s="103"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="103"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="103"/>
+      <c r="M26" s="103"/>
+      <c r="N26" s="103"/>
+      <c r="O26" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
+      <c r="S26" s="84"/>
       <c r="T26" s="21"/>
       <c r="U26" s="14"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" s="39"/>
+      <c r="A27" s="103"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="103"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
       <c r="O27" s="19"/>
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
@@ -2338,10 +2234,10 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="P28" s="42"/>
+      <c r="O28" s="106" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="106"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="8"/>
@@ -2395,88 +2291,68 @@
       <c r="U30" s="14"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="N31" s="40"/>
-      <c r="O31" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="86"/>
+      <c r="P31" s="86"/>
+      <c r="Q31" s="86"/>
+      <c r="R31" s="86"/>
+      <c r="S31" s="86"/>
       <c r="T31" s="21"/>
       <c r="U31" s="14"/>
     </row>
-    <row r="32" spans="1:21" ht="18.75">
-      <c r="A32" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="39"/>
-      <c r="S32" s="39"/>
+    <row r="32" spans="1:21">
+      <c r="A32" s="103"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="103"/>
+      <c r="K32" s="103"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="103" t="s">
+        <v>25</v>
+      </c>
+      <c r="P32" s="103"/>
+      <c r="Q32" s="103"/>
+      <c r="R32" s="103"/>
+      <c r="S32" s="103"/>
       <c r="T32" s="21"/>
       <c r="U32" s="14"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="N33" s="39"/>
+      <c r="A33" s="103"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
+      <c r="J33" s="103"/>
+      <c r="K33" s="103"/>
+      <c r="L33" s="103"/>
+      <c r="M33" s="103"/>
+      <c r="N33" s="103"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -2552,23 +2428,52 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="24" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="O32:S32"/>
+    <mergeCell ref="O31:S31"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="G3:K4"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="A1:S2"/>
     <mergeCell ref="O22:S22"/>
@@ -2585,47 +2490,18 @@
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="I12:I15"/>
     <mergeCell ref="A10:H11"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="G3:K4"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="I33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="I32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="O32:S32"/>
-    <mergeCell ref="O31:S31"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="S10:S11"/>
   </mergeCells>
   <conditionalFormatting sqref="O11:Q11">
     <cfRule type="expression" dxfId="11" priority="21">
@@ -2652,14 +2528,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0546A6F-3D66-409E-AB7A-9126D06267A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2687,63 +2563,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
       <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
@@ -2753,13 +2629,13 @@
       <c r="N3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="9"/>
@@ -2768,65 +2644,65 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
       <c r="L4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="M4" s="30"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
+      <c r="A5" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
       <c r="L6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
       <c r="O6" s="5"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="5"/>
@@ -2834,24 +2710,24 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
       <c r="L7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -2872,7 +2748,7 @@
       <c r="K8" s="38"/>
       <c r="L8" s="7"/>
       <c r="M8" s="10" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="N8" s="30"/>
       <c r="O8" s="5"/>
@@ -2903,103 +2779,103 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="1:21" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="53" t="s">
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="55" t="s">
+      <c r="J10" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="53" t="s">
+      <c r="K10" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="49"/>
-      <c r="O10" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" s="53" t="s">
+      <c r="M10" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="70"/>
+      <c r="O10" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="T10" s="59" t="s">
+      <c r="T10" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="U10" s="61" t="s">
+      <c r="U10" s="65" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="26.25" thickBot="1">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="52"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="72"/>
       <c r="O11" s="11" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="62"/>
+        <v>32</v>
+      </c>
+      <c r="R11" s="68"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="66"/>
     </row>
     <row r="12" spans="1:21" s="35" customFormat="1">
       <c r="A12" s="33">
         <v>1</v>
       </c>
       <c r="B12" s="34"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="75"/>
-      <c r="T12" s="76"/>
-      <c r="U12" s="77"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="93"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="45"/>
     </row>
     <row r="13" spans="1:21" s="35" customFormat="1">
       <c r="A13" s="36"/>
@@ -3007,27 +2883,27 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="87"/>
-      <c r="Q13" s="87"/>
-      <c r="R13" s="87"/>
-      <c r="S13" s="88"/>
-      <c r="T13" s="89"/>
-      <c r="U13" s="90"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="52"/>
+      <c r="U13" s="53"/>
     </row>
     <row r="14" spans="1:21" s="35" customFormat="1">
       <c r="A14" s="36"/>
@@ -3035,27 +2911,27 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="87"/>
-      <c r="Q14" s="87"/>
-      <c r="R14" s="87"/>
-      <c r="S14" s="88"/>
-      <c r="T14" s="89"/>
-      <c r="U14" s="91"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="54"/>
     </row>
     <row r="15" spans="1:21" s="35" customFormat="1">
       <c r="A15" s="36"/>
@@ -3063,50 +2939,50 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="85"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87"/>
-      <c r="R15" s="87"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="91"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="52"/>
+      <c r="U15" s="54"/>
     </row>
     <row r="16" spans="1:21" s="35" customFormat="1">
       <c r="A16" s="36"/>
       <c r="B16" s="37"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="84"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="86"/>
-      <c r="P16" s="87"/>
-      <c r="Q16" s="87"/>
-      <c r="R16" s="87"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="89"/>
-      <c r="U16" s="91"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="88"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="52"/>
+      <c r="U16" s="54"/>
     </row>
     <row r="17" spans="1:21" ht="16.5" thickBot="1">
       <c r="A17" s="32"/>
@@ -3114,25 +2990,25 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="97"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="99"/>
-      <c r="M17" s="100"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="105"/>
-      <c r="U17" s="106"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="61"/>
+      <c r="U17" s="62"/>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="5" t="s">
@@ -3242,13 +3118,13 @@
       <c r="L22" s="10"/>
       <c r="M22" s="13"/>
       <c r="N22" s="5"/>
-      <c r="O22" s="41" t="s">
+      <c r="O22" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="84"/>
+      <c r="R22" s="84"/>
+      <c r="S22" s="84"/>
       <c r="U22" s="14"/>
     </row>
     <row r="23" spans="1:21">
@@ -3271,26 +3147,20 @@
       <c r="U23" s="14"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="N24" s="40"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="86"/>
       <c r="O24" s="19"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
@@ -3299,26 +3169,20 @@
       <c r="U24" s="14"/>
     </row>
     <row r="25" spans="1:21" ht="16.5" thickBot="1">
-      <c r="A25" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="N25" s="39"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="103"/>
+      <c r="J25" s="103"/>
+      <c r="K25" s="103"/>
+      <c r="L25" s="103"/>
+      <c r="M25" s="103"/>
+      <c r="N25" s="103"/>
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="20"/>
@@ -3328,57 +3192,45 @@
       <c r="U25" s="14"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="N26" s="39"/>
-      <c r="O26" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
+      <c r="A26" s="103"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="103"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="103"/>
+      <c r="M26" s="103"/>
+      <c r="N26" s="103"/>
+      <c r="O26" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
+      <c r="S26" s="84"/>
       <c r="T26" s="21"/>
       <c r="U26" s="14"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" s="39"/>
+      <c r="A27" s="103"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="103"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
       <c r="O27" s="19"/>
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
@@ -3402,10 +3254,10 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="P28" s="42"/>
+      <c r="O28" s="106" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="106"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="8"/>
@@ -3459,88 +3311,68 @@
       <c r="U30" s="14"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="N31" s="40"/>
-      <c r="O31" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="86"/>
+      <c r="P31" s="86"/>
+      <c r="Q31" s="86"/>
+      <c r="R31" s="86"/>
+      <c r="S31" s="86"/>
       <c r="T31" s="21"/>
       <c r="U31" s="14"/>
     </row>
-    <row r="32" spans="1:21" ht="18.75">
-      <c r="A32" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="39"/>
-      <c r="S32" s="39"/>
+    <row r="32" spans="1:21">
+      <c r="A32" s="103"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="103"/>
+      <c r="K32" s="103"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="103" t="s">
+        <v>25</v>
+      </c>
+      <c r="P32" s="103"/>
+      <c r="Q32" s="103"/>
+      <c r="R32" s="103"/>
+      <c r="S32" s="103"/>
       <c r="T32" s="21"/>
       <c r="U32" s="14"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="N33" s="39"/>
+      <c r="A33" s="103"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
+      <c r="J33" s="103"/>
+      <c r="K33" s="103"/>
+      <c r="L33" s="103"/>
+      <c r="M33" s="103"/>
+      <c r="N33" s="103"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -3616,26 +3448,49 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="24" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="A1:S2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="O3:U3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="O5:U5"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="A10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="M25:N25"/>
     <mergeCell ref="A33:H33"/>
     <mergeCell ref="I33:L33"/>
     <mergeCell ref="M33:N33"/>
@@ -3652,44 +3507,21 @@
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="I26:L26"/>
     <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="A1:S2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="O3:U3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="O5:U5"/>
-    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="O10:Q10"/>
   </mergeCells>
   <conditionalFormatting sqref="O11:Q11">
     <cfRule type="expression" dxfId="7" priority="25">
@@ -3716,14 +3548,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB385367-FBE7-4937-BFF1-6A1339DBB179}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3751,63 +3583,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
       <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
@@ -3817,13 +3649,13 @@
       <c r="N3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="9"/>
@@ -3832,65 +3664,65 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
       <c r="L4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="M4" s="30"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
+      <c r="A5" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
       <c r="L6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
       <c r="O6" s="5"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="5"/>
@@ -3898,24 +3730,24 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
       <c r="L7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -3936,7 +3768,7 @@
       <c r="K8" s="38"/>
       <c r="L8" s="7"/>
       <c r="M8" s="10" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="N8" s="30"/>
       <c r="O8" s="5"/>
@@ -3967,103 +3799,103 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="1:21" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="53" t="s">
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="55" t="s">
+      <c r="J10" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="53" t="s">
+      <c r="K10" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="49"/>
-      <c r="O10" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" s="53" t="s">
+      <c r="M10" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="70"/>
+      <c r="O10" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="T10" s="59" t="s">
+      <c r="T10" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="U10" s="61" t="s">
+      <c r="U10" s="65" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="26.25" thickBot="1">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="52"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="72"/>
       <c r="O11" s="11" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="62"/>
+        <v>32</v>
+      </c>
+      <c r="R11" s="68"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="66"/>
     </row>
     <row r="12" spans="1:21" s="35" customFormat="1">
       <c r="A12" s="33">
         <v>1</v>
       </c>
       <c r="B12" s="34"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="75"/>
-      <c r="T12" s="76"/>
-      <c r="U12" s="77"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="93"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="45"/>
     </row>
     <row r="13" spans="1:21" s="35" customFormat="1">
       <c r="A13" s="36"/>
@@ -4071,27 +3903,27 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="87"/>
-      <c r="Q13" s="87"/>
-      <c r="R13" s="87"/>
-      <c r="S13" s="88"/>
-      <c r="T13" s="89"/>
-      <c r="U13" s="90"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="52"/>
+      <c r="U13" s="53"/>
     </row>
     <row r="14" spans="1:21" s="35" customFormat="1">
       <c r="A14" s="36"/>
@@ -4099,27 +3931,27 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="87"/>
-      <c r="Q14" s="87"/>
-      <c r="R14" s="87"/>
-      <c r="S14" s="88"/>
-      <c r="T14" s="89"/>
-      <c r="U14" s="91"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="54"/>
     </row>
     <row r="15" spans="1:21" s="35" customFormat="1">
       <c r="A15" s="36"/>
@@ -4127,50 +3959,50 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="85"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87"/>
-      <c r="R15" s="87"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="91"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="52"/>
+      <c r="U15" s="54"/>
     </row>
     <row r="16" spans="1:21" s="35" customFormat="1">
       <c r="A16" s="36"/>
       <c r="B16" s="37"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="84"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="86"/>
-      <c r="P16" s="87"/>
-      <c r="Q16" s="87"/>
-      <c r="R16" s="87"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="89"/>
-      <c r="U16" s="91"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="88"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="52"/>
+      <c r="U16" s="54"/>
     </row>
     <row r="17" spans="1:21" ht="16.5" thickBot="1">
       <c r="A17" s="32"/>
@@ -4178,25 +4010,25 @@
         <f>B12</f>
         <v>0</v>
       </c>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="97"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="99"/>
-      <c r="M17" s="100"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="103"/>
-      <c r="Q17" s="103"/>
-      <c r="R17" s="103"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="105"/>
-      <c r="U17" s="106"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="61"/>
+      <c r="U17" s="62"/>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="5" t="s">
@@ -4306,13 +4138,13 @@
       <c r="L22" s="10"/>
       <c r="M22" s="13"/>
       <c r="N22" s="5"/>
-      <c r="O22" s="41" t="s">
+      <c r="O22" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="84"/>
+      <c r="R22" s="84"/>
+      <c r="S22" s="84"/>
       <c r="U22" s="14"/>
     </row>
     <row r="23" spans="1:21">
@@ -4335,26 +4167,20 @@
       <c r="U23" s="14"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="N24" s="40"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="86"/>
       <c r="O24" s="19"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
@@ -4363,26 +4189,20 @@
       <c r="U24" s="14"/>
     </row>
     <row r="25" spans="1:21" ht="16.5" thickBot="1">
-      <c r="A25" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="N25" s="39"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="103"/>
+      <c r="J25" s="103"/>
+      <c r="K25" s="103"/>
+      <c r="L25" s="103"/>
+      <c r="M25" s="103"/>
+      <c r="N25" s="103"/>
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="20"/>
@@ -4392,57 +4212,45 @@
       <c r="U25" s="14"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="N26" s="39"/>
-      <c r="O26" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
+      <c r="A26" s="103"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="103"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="103"/>
+      <c r="M26" s="103"/>
+      <c r="N26" s="103"/>
+      <c r="O26" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
+      <c r="S26" s="84"/>
       <c r="T26" s="21"/>
       <c r="U26" s="14"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" s="39"/>
+      <c r="A27" s="103"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="103"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
       <c r="O27" s="19"/>
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
@@ -4466,10 +4274,10 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="P28" s="42"/>
+      <c r="O28" s="106" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="106"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="8"/>
@@ -4523,88 +4331,68 @@
       <c r="U30" s="14"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="N31" s="40"/>
-      <c r="O31" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="86"/>
+      <c r="P31" s="86"/>
+      <c r="Q31" s="86"/>
+      <c r="R31" s="86"/>
+      <c r="S31" s="86"/>
       <c r="T31" s="21"/>
       <c r="U31" s="14"/>
     </row>
-    <row r="32" spans="1:21" ht="18.75">
-      <c r="A32" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="39"/>
-      <c r="S32" s="39"/>
+    <row r="32" spans="1:21">
+      <c r="A32" s="103"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="103"/>
+      <c r="K32" s="103"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="103" t="s">
+        <v>25</v>
+      </c>
+      <c r="P32" s="103"/>
+      <c r="Q32" s="103"/>
+      <c r="R32" s="103"/>
+      <c r="S32" s="103"/>
       <c r="T32" s="21"/>
       <c r="U32" s="14"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="N33" s="39"/>
+      <c r="A33" s="103"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
+      <c r="J33" s="103"/>
+      <c r="K33" s="103"/>
+      <c r="L33" s="103"/>
+      <c r="M33" s="103"/>
+      <c r="N33" s="103"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -4680,26 +4468,49 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="24" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="A1:S2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="O3:U3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="O5:U5"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="A10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="M25:N25"/>
     <mergeCell ref="A33:H33"/>
     <mergeCell ref="I33:L33"/>
     <mergeCell ref="M33:N33"/>
@@ -4716,44 +4527,21 @@
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="I26:L26"/>
     <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="A1:S2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="O3:U3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="O5:U5"/>
-    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="O10:Q10"/>
   </mergeCells>
   <conditionalFormatting sqref="O11:Q11">
     <cfRule type="expression" dxfId="3" priority="23">

</xml_diff>